<commit_message>
Added more detail to the spreadsheet.
</commit_message>
<xml_diff>
--- a/ResponseAndSummaryOfChanges.xlsx
+++ b/ResponseAndSummaryOfChanges.xlsx
@@ -101,7 +101,7 @@
   </si>
   <si>
     <t xml:space="preserve">We have rewritten the introduction to more clearly expose the
-Motivation and to better captivate the audience.</t>
+motivation and to better captivate the audience. The words “this project” no longer appear. The introduction now begins with a general commentary on how different environmental effects complicate analysis and how the different effects leaves designers decreasing impacts in one dimension while increasing it another one. It then proceeds to explain how designers can use weighting techniques to assess multiple impacts at once and how this technique complicates assessments. Finally, the introduction presents a specific pair of products to use in a case study on how weighting might dictate design practices.</t>
   </si>
   <si>
     <t xml:space="preserve">Ok, you took care of this by rewriting the intro</t>
@@ -111,8 +111,7 @@
   </si>
   <si>
     <t xml:space="preserve">The introduction now contains a more elaborate justification for the
-weighting triangle on page 2 in the second paragraph. It no longer
-references tradition.</t>
+weighting triangle on page 2 where it explains how the study concerns the most common analysis practices and how SimaPro, which utilizes the weighting triangle, is one of the two most common software packages used. We do not use tradition to try to justify anything.</t>
   </si>
   <si>
     <t xml:space="preserve">True, but that's more a problem of phrasing as we just need to include the justification. Instead of "others found it useful and therefore we follow the tradition", it may make sense to state "as [A,B,C] have successfully applied a weighting triangle to investigate X and Y, we decided to also use it as our questions lend themselves, but this is already fixed in the new version.</t>
@@ -130,8 +129,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">We have reduced the number of introductions of the weighting factor.
-The introduction now contains a clarification of the LCIA on page 2 in
-the fourth paragraph. We stress that LCIA does </t>
+Also, the introduction now contains a clarification of the LCIA on page 2 We stress that LCIA does </t>
     </r>
     <r>
       <rPr>
@@ -152,9 +150,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> amount to 
-LCA + Eco-indicator 99. It only refers to Eco-Indicator 99, which is 
-one  method available for implementing the LCIA.</t>
+      <t xml:space="preserve"> amount to  LCA + Eco-indicator 99. It only refers to an axuliary phase of the LCA, and Eco-Indicator 99 is one  method available for implementing the LCIA. We believe the new explanation makes clearer what LCIA is and how it relates to the overall LCA and Eco-indicator 99.</t>
     </r>
   </si>
   <si>
@@ -223,7 +219,7 @@
   </si>
   <si>
     <t xml:space="preserve">The introduction now has a justification for LCA and Eco-Indicator 99
-based on their prevalence in practice and their accessability.</t>
+based on their prevalence and our intention to focus on common practices. We emphasize the data limitations to make the reader aware of the study’s limitations, but the methodologies in this paper need not use these particular data. We use these data because of their availability given our limited resources, but they are not inherent to our methodogies. However, we concede that the data introduce uncertainties to our results. We could not eliminate all of the limitations in our work.</t>
   </si>
   <si>
     <t xml:space="preserve">Ok, need to check if justifications are now given.</t>
@@ -232,7 +228,7 @@
     <t xml:space="preserve">4. The example of compact fluorescent lamps majorly occupies the abstract and shows no relevance or connection to title and keywords. </t>
   </si>
   <si>
-    <t xml:space="preserve">The abstract no longer mentions cfls.</t>
+    <t xml:space="preserve">The abstract no longer mentions cfls, which now focuses on the paper’s central case study. We only mention the cfls in the introduction as an example of the tradeoffs in green technology.</t>
   </si>
   <si>
     <t xml:space="preserve">Oh, right, the lamps were an initial motivating example but they are not the central point of the article.</t>
@@ -242,8 +238,7 @@
   </si>
   <si>
     <t xml:space="preserve">The use hours reference now appears in the same sentence in which
-we first reference use hours on page 6, second paragraph from the
-Bottom in the right column.</t>
+we first reference use hours, “The desktop computers have more use hours because, in practice, users usually switch off thin clients at night, but only 30% of users switch off desktop computers [2].”</t>
   </si>
   <si>
     <t xml:space="preserve">OK, need to make sure all statements are justified and/or referenced.</t>
@@ -287,9 +282,9 @@
   <si>
     <t xml:space="preserve">We use information from databases.
 I think the reviewer has suggested
-that we get our own number from
+that we get our own numbers from
 measuring material instead of using
-the databases. I see no plausible
+the databases. I see no realistic
 way to satisfy this recommendation.</t>
   </si>
   <si>
@@ -317,8 +312,7 @@
 know if it would add anything to the
 paper. I didn’t do anything unique
 with the LCA and followed the
-official documentation as closely as I
-Could, so I don’t think we have
+official documentation as closely as I could, so I don’t think we have
 anything to say about how our
 method differs from existing LCAs.</t>
   </si>
@@ -775,8 +769,8 @@
   </sheetPr>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A120" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B126" activeCellId="0" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,7 +904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>25</v>
       </c>
@@ -1039,7 +1033,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
         <v>53</v>
       </c>
@@ -1050,7 +1044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
         <v>56</v>
       </c>
@@ -1061,7 +1055,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
         <v>59</v>
       </c>

</xml_diff>